<commit_message>
Chkd & Updated ic fd
</commit_message>
<xml_diff>
--- a/Fix/fix cur. 20.xlsx
+++ b/Fix/fix cur. 20.xlsx
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="32" spans="1:21" ht="12.75" customHeight="1">
       <c r="A32" s="44">
-        <v>41941</v>
+        <v>41947</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="3"/>

</xml_diff>

<commit_message>
Updated sb ren and hd mat
</commit_message>
<xml_diff>
--- a/Fix/fix cur. 20.xlsx
+++ b/Fix/fix cur. 20.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t>amt</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>1111500111463301</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50300020863891 </t>
   </si>
   <si>
     <t>1111500111466401</t>
@@ -269,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -356,22 +353,9 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -416,6 +400,22 @@
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U108"/>
+  <dimension ref="A1:U107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -873,47 +873,47 @@
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
     </row>
-    <row r="3" spans="1:21" s="37" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A3" s="32">
+    <row r="3" spans="1:21" s="54" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A3" s="49">
         <v>10.75</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="49">
         <v>9.25</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="49">
         <v>1</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="33">
+      <c r="F3" s="49"/>
+      <c r="G3" s="50">
         <v>41636</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="50">
         <v>42001</v>
       </c>
-      <c r="I3" s="34">
+      <c r="I3" s="51">
         <f>24188/3</f>
         <v>8062.666666666667</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
     </row>
     <row r="4" spans="1:21" s="12" customFormat="1" ht="12.75" customHeight="1">
       <c r="A4" s="9">
@@ -931,7 +931,7 @@
       <c r="E4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="52"/>
+      <c r="F4" s="47"/>
       <c r="G4" s="15">
         <v>41713</v>
       </c>
@@ -956,87 +956,87 @@
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
     </row>
-    <row r="5" spans="1:21" s="50" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A5" s="46">
+    <row r="5" spans="1:21" s="12" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A5" s="9">
+        <v>6.75</v>
+      </c>
+      <c r="B5" s="9">
+        <v>9.25</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="15">
+        <v>41887</v>
+      </c>
+      <c r="H5" s="15">
+        <v>42252</v>
+      </c>
+      <c r="I5" s="19">
+        <v>5164</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="9"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+    </row>
+    <row r="6" spans="1:21" s="45" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A6" s="41">
         <v>1.5</v>
       </c>
-      <c r="B5" s="46">
-        <v>9.75</v>
-      </c>
-      <c r="C5" s="46">
+      <c r="B6" s="41">
+        <v>9</v>
+      </c>
+      <c r="C6" s="41">
         <v>1000</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D6" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E6" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="51">
-        <v>40941</v>
-      </c>
-      <c r="H5" s="51">
+      <c r="F6" s="41"/>
+      <c r="G6" s="46">
         <v>41941</v>
       </c>
-      <c r="I5" s="47">
-        <v>1209</v>
-      </c>
-      <c r="J5" s="48" t="s">
+      <c r="H6" s="46">
+        <v>42941</v>
+      </c>
+      <c r="I6" s="42">
+        <v>1073</v>
+      </c>
+      <c r="J6" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="46"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="49"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="49"/>
-      <c r="U5" s="49"/>
-    </row>
-    <row r="6" spans="1:21" s="12" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="9">
-        <v>6.75</v>
-      </c>
-      <c r="B6" s="9">
-        <v>9.25</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="15">
-        <v>41887</v>
-      </c>
-      <c r="H6" s="15">
-        <v>42252</v>
-      </c>
-      <c r="I6" s="19">
-        <v>5164</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="44"/>
     </row>
     <row r="7" spans="1:21" ht="12.75" customHeight="1">
       <c r="A7" s="3"/>
@@ -1052,8 +1052,8 @@
       <c r="H7" s="3"/>
       <c r="I7" s="8"/>
       <c r="K7" s="8">
-        <f>SUM(I3:I6)</f>
-        <v>17877.666666666668</v>
+        <f>SUM(I3:I5)</f>
+        <v>16668.666666666668</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -1089,7 +1089,7 @@
       <c r="H8" s="21">
         <v>42399</v>
       </c>
-      <c r="I8" s="53">
+      <c r="I8" s="48">
         <v>10215</v>
       </c>
       <c r="J8" s="10" t="s">
@@ -1175,7 +1175,7 @@
         <v>3425</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="11"/>
@@ -1216,7 +1216,7 @@
         <v>2309</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="11"/>
@@ -1267,13 +1267,13 @@
         <v>9.6</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="15">
@@ -1314,7 +1314,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="15">
@@ -1327,7 +1327,7 @@
         <v>10125</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="11"/>
@@ -1355,7 +1355,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="15">
@@ -1368,7 +1368,7 @@
         <v>3175</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="11"/>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="19" spans="1:21" s="12" customFormat="1" ht="12.75" customHeight="1">
       <c r="A19" s="9">
-        <v>2.9</v>
+        <v>11.9</v>
       </c>
       <c r="B19" s="9">
         <v>9.43</v>
@@ -1511,16 +1511,16 @@
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="15">
-        <v>41589</v>
+        <v>41673</v>
       </c>
       <c r="H19" s="15">
-        <v>41955</v>
+        <v>42039</v>
       </c>
       <c r="I19" s="19">
-        <v>2322</v>
+        <v>9531</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="11"/>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="20" spans="1:21" s="12" customFormat="1" ht="12.75" customHeight="1">
       <c r="A20" s="9">
-        <v>11.9</v>
+        <v>3.55</v>
       </c>
       <c r="B20" s="9">
         <v>9.43</v>
@@ -1552,16 +1552,16 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="15">
-        <v>41673</v>
+        <v>41761</v>
       </c>
       <c r="H20" s="15">
-        <v>42039</v>
-      </c>
-      <c r="I20" s="19">
-        <v>9531</v>
+        <v>42127</v>
+      </c>
+      <c r="I20" s="31">
+        <v>2843</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="11"/>
@@ -1575,126 +1575,126 @@
       <c r="T20" s="11"/>
       <c r="U20" s="11"/>
     </row>
-    <row r="21" spans="1:21" s="12" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A21" s="9">
-        <v>3.55</v>
-      </c>
-      <c r="B21" s="9">
-        <v>9.43</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="9" t="s">
+    <row r="21" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <f>SUM(A17:A20)</f>
+        <v>22.150000000000002</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="8">
+        <f>SUM(I17:I20)</f>
+        <v>17598</v>
+      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+    </row>
+    <row r="22" spans="1:21" s="12" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A22" s="9">
+        <v>2.4</v>
+      </c>
+      <c r="B22" s="9">
+        <v>10</v>
+      </c>
+      <c r="C22" s="9">
+        <v>2</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="15">
-        <v>41761</v>
-      </c>
-      <c r="H21" s="15">
-        <v>42127</v>
-      </c>
-      <c r="I21" s="31">
-        <v>2843</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-    </row>
-    <row r="22" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3">
-        <f>SUM(A17:A21)</f>
-        <v>25.05</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="8">
-        <f>SUM(I17:I21)</f>
-        <v>19920</v>
-      </c>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-    </row>
-    <row r="23" spans="1:21" s="12" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A23" s="9">
-        <v>2.4</v>
-      </c>
-      <c r="B23" s="9">
-        <v>10</v>
-      </c>
-      <c r="C23" s="9">
-        <v>2</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="E22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="15">
+        <v>41637</v>
+      </c>
+      <c r="H22" s="15">
+        <v>42367</v>
+      </c>
+      <c r="I22" s="19">
+        <v>2000</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="9"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+    </row>
+    <row r="23" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A23" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="B23" s="3">
+        <v>9.75</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="15">
-        <v>41637</v>
-      </c>
-      <c r="H23" s="15">
-        <v>42367</v>
+      <c r="F23" s="3"/>
+      <c r="G23" s="5">
+        <v>41405</v>
+      </c>
+      <c r="H23" s="5">
+        <v>42105</v>
       </c>
       <c r="I23" s="19">
-        <v>2000</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K23" s="9"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
+        <v>3169</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
     </row>
     <row r="24" spans="1:21" ht="12.75" customHeight="1">
       <c r="A24" s="3">
-        <v>3.9</v>
+        <v>3.45</v>
       </c>
       <c r="B24" s="3">
         <v>9.75</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>25</v>
+      <c r="C24" s="3">
+        <v>2</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>6</v>
@@ -1704,16 +1704,16 @@
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="5">
-        <v>41405</v>
+        <v>41429</v>
       </c>
       <c r="H24" s="5">
-        <v>42105</v>
+        <v>42159</v>
       </c>
       <c r="I24" s="19">
-        <v>3169</v>
+        <v>2803</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="4"/>
@@ -1729,7 +1729,7 @@
     </row>
     <row r="25" spans="1:21" ht="12.75" customHeight="1">
       <c r="A25" s="3">
-        <v>3.45</v>
+        <v>5.75</v>
       </c>
       <c r="B25" s="3">
         <v>9.75</v>
@@ -1745,16 +1745,16 @@
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="5">
-        <v>41429</v>
+        <v>41520</v>
       </c>
       <c r="H25" s="5">
-        <v>42159</v>
+        <v>42250</v>
       </c>
       <c r="I25" s="19">
-        <v>2803</v>
+        <v>4672</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="4"/>
@@ -1768,9 +1768,9 @@
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
     </row>
-    <row r="26" spans="1:21" ht="12.75" customHeight="1">
+    <row r="26" spans="1:21" s="27" customFormat="1" ht="12.75" customHeight="1">
       <c r="A26" s="3">
-        <v>5.75</v>
+        <v>3.15</v>
       </c>
       <c r="B26" s="3">
         <v>9.75</v>
@@ -1786,32 +1786,32 @@
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="5">
-        <v>41520</v>
+        <v>41536</v>
       </c>
       <c r="H26" s="5">
-        <v>42250</v>
+        <v>42266</v>
       </c>
       <c r="I26" s="19">
-        <v>4672</v>
+        <v>2559</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-    </row>
-    <row r="27" spans="1:21" s="27" customFormat="1" ht="12.75" customHeight="1">
+        <v>31</v>
+      </c>
+      <c r="K26" s="25"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+    </row>
+    <row r="27" spans="1:21" ht="12.75" customHeight="1">
       <c r="A27" s="3">
-        <v>3.15</v>
+        <v>4.5</v>
       </c>
       <c r="B27" s="3">
         <v>9.75</v>
@@ -1827,111 +1827,99 @@
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="5">
-        <v>41536</v>
+        <v>41552</v>
       </c>
       <c r="H27" s="5">
-        <v>42266</v>
+        <v>42282</v>
       </c>
       <c r="I27" s="19">
-        <v>2559</v>
+        <v>3656</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K27" s="25"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="26"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="26"/>
-    </row>
-    <row r="28" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A28" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="B28" s="3">
-        <v>9.75</v>
-      </c>
-      <c r="C28" s="3">
-        <v>2</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="K27" s="3"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+    </row>
+    <row r="28" spans="1:21" s="37" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A28" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="B28" s="33">
+        <v>9</v>
+      </c>
+      <c r="C28" s="33">
+        <v>60</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="5">
-        <v>41552</v>
-      </c>
-      <c r="H28" s="5">
-        <v>42282</v>
-      </c>
-      <c r="I28" s="19">
-        <v>3656</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K28" s="3"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-    </row>
-    <row r="29" spans="1:21" s="42" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A29" s="38">
-        <v>0.5</v>
-      </c>
-      <c r="B29" s="38">
-        <v>9</v>
-      </c>
-      <c r="C29" s="38">
-        <v>60</v>
-      </c>
-      <c r="D29" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="38"/>
-      <c r="G29" s="39">
+      <c r="F28" s="33"/>
+      <c r="G28" s="34">
         <v>41650</v>
       </c>
-      <c r="H29" s="39">
+      <c r="H28" s="34">
         <v>43476</v>
       </c>
-      <c r="I29" s="34">
+      <c r="I28" s="32">
         <f>1125/3</f>
         <v>375</v>
       </c>
-      <c r="J29" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="K29" s="38"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="41"/>
-      <c r="S29" s="41"/>
-      <c r="T29" s="41"/>
-      <c r="U29" s="41"/>
+      <c r="J28" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="K28" s="33"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="36"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="36"/>
+      <c r="R28" s="36"/>
+      <c r="S28" s="36"/>
+      <c r="T28" s="36"/>
+      <c r="U28" s="36"/>
+    </row>
+    <row r="29" spans="1:21" ht="12.75" customHeight="1">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3">
+        <f>SUM(A22:A28)</f>
+        <v>23.65</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="8">
+        <f>SUM(I22:I27)</f>
+        <v>18859</v>
+      </c>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
     </row>
     <row r="30" spans="1:21" ht="12.75" customHeight="1">
       <c r="A30" s="3"/>
@@ -1939,18 +1927,12 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="3">
-        <f>SUM(A23:A29)</f>
-        <v>23.65</v>
-      </c>
+      <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="8"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="8">
-        <f>SUM(I23:I28)</f>
-        <v>18859</v>
-      </c>
+      <c r="K30" s="3"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -1963,16 +1945,26 @@
       <c r="U30" s="4"/>
     </row>
     <row r="31" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
+      <c r="A31" s="39">
+        <v>41967</v>
+      </c>
+      <c r="B31" s="8"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="F31" s="1">
+        <f>SUM(F3:F29)</f>
+        <v>115.35000000000002</v>
+      </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="3"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="16">
+        <f>SUM(I3:I27)</f>
+        <v>91452.666666666672</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="K31" s="3"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
@@ -1986,26 +1978,16 @@
       <c r="U31" s="4"/>
     </row>
     <row r="32" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A32" s="44">
-        <v>41947</v>
-      </c>
+      <c r="A32" s="3"/>
       <c r="B32" s="8"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="1">
-        <f>SUM(F3:F30)</f>
-        <v>118.25</v>
-      </c>
+      <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="16">
-        <f>SUM(I3:I28)</f>
-        <v>93910.666666666672</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>3</v>
-      </c>
+      <c r="H32" s="3"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
@@ -2021,14 +2003,18 @@
     <row r="33" spans="1:21" ht="12.75" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="8"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="3"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="8">
+        <v>18095</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="K33" s="3"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -2043,19 +2029,14 @@
     </row>
     <row r="34" spans="1:21" ht="12.75" customHeight="1">
       <c r="A34" s="3"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
+      <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="8">
-        <v>18095</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I34" s="20"/>
+      <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -2070,13 +2051,19 @@
     </row>
     <row r="35" spans="1:21" ht="12.75" customHeight="1">
       <c r="A35" s="3"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="G35">
+        <v>400000</v>
+      </c>
       <c r="H35" s="4"/>
-      <c r="I35" s="20"/>
+      <c r="I35" s="17">
+        <f>I31+I33</f>
+        <v>109547.66666666667</v>
+      </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="4"/>
@@ -2091,20 +2078,15 @@
       <c r="U35" s="4"/>
     </row>
     <row r="36" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A36" s="3"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="14"/>
       <c r="G36">
-        <v>400000</v>
+        <v>285000</v>
       </c>
       <c r="H36" s="4"/>
-      <c r="I36" s="17">
-        <f>I32+I34</f>
-        <v>112005.66666666667</v>
-      </c>
+      <c r="I36" s="4"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="4"/>
@@ -2121,11 +2103,8 @@
     <row r="37" spans="1:21" ht="12.75" customHeight="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="14"/>
-      <c r="G37">
-        <v>285000</v>
-      </c>
+      <c r="C37" s="12"/>
+      <c r="E37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="3"/>
@@ -2144,11 +2123,14 @@
     <row r="38" spans="1:21" ht="12.75" customHeight="1">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
-      <c r="C38" s="12"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
       <c r="E38" s="4"/>
-      <c r="H38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="8"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="3"/>
+      <c r="J38" s="40"/>
       <c r="K38" s="3"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
@@ -2162,16 +2144,24 @@
       <c r="U38" s="4"/>
     </row>
     <row r="39" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
+      <c r="A39" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C39" s="4">
+        <f>SUM(I22:I27) * 12 + 4*I28</f>
+        <v>227808</v>
+      </c>
+      <c r="E39" s="4">
+        <f>B39-C39</f>
+        <v>22192</v>
+      </c>
       <c r="G39" s="4"/>
-      <c r="H39" s="8"/>
+      <c r="H39" s="4"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="45"/>
+      <c r="J39" s="40"/>
       <c r="K39" s="3"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -2192,17 +2182,17 @@
         <v>250000</v>
       </c>
       <c r="C40" s="4">
-        <f>SUM(I23:I28) * 12 + 4*I29</f>
-        <v>227808</v>
+        <f>SUM(I17:I20) * 12</f>
+        <v>211176</v>
       </c>
       <c r="E40" s="4">
         <f>B40-C40</f>
-        <v>22192</v>
+        <v>38824</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="45"/>
+      <c r="J40" s="40"/>
       <c r="K40" s="3"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -2223,17 +2213,30 @@
         <v>250000</v>
       </c>
       <c r="C41" s="4">
-        <f>SUM(I17:I21) * 12</f>
-        <v>239040</v>
-      </c>
+        <f>(29597 + 6488) + (3175 * 2 + 1258) + (3175 * 12) + (5354 * 3 + 1040) + (6075 + 10125 * 11) + (1331 + 3175 * 8)</f>
+        <v>243076</v>
+      </c>
+      <c r="D41" s="4"/>
       <c r="E41" s="4">
-        <f>B41-C41</f>
-        <v>10960</v>
-      </c>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="45"/>
+        <f t="shared" ref="E41:E43" si="0">B41-C41</f>
+        <v>6924</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41">
+        <f>G35*0.1/12</f>
+        <v>3333.3333333333335</v>
+      </c>
+      <c r="H41" s="20">
+        <v>9</v>
+      </c>
+      <c r="I41" s="20">
+        <f>G41*H41</f>
+        <v>30000</v>
+      </c>
+      <c r="J41" s="38">
+        <f>C41+I41</f>
+        <v>273076</v>
+      </c>
       <c r="K41" s="3"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -2254,29 +2257,29 @@
         <v>250000</v>
       </c>
       <c r="C42" s="4">
-        <f>(29597 + 6488) + (3175 * 2 + 1258) + (3175 * 12) + (5354 * 3 + 1040) + (6075 + 10125 * 11) + (1331 + 3175 * 8)</f>
-        <v>243076</v>
+        <f>(4030 * 3) + (3425 * 9) + (10215 * 12) + (4830 * 12) + 567 + (2309 * 9)</f>
+        <v>244803</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4">
-        <f t="shared" ref="E42:E44" si="0">B42-C42</f>
-        <v>6924</v>
+        <f>B42-C42</f>
+        <v>5197</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42">
         <f>G36*0.1/12</f>
-        <v>3333.3333333333335</v>
+        <v>2375</v>
       </c>
       <c r="H42" s="20">
         <v>9</v>
       </c>
       <c r="I42" s="20">
         <f>G42*H42</f>
-        <v>30000</v>
-      </c>
-      <c r="J42" s="43">
+        <v>21375</v>
+      </c>
+      <c r="J42" s="38">
         <f>C42+I42</f>
-        <v>273076</v>
+        <v>266178</v>
       </c>
       <c r="K42" s="3"/>
       <c r="L42" s="4"/>
@@ -2298,30 +2301,19 @@
         <v>250000</v>
       </c>
       <c r="C43" s="4">
-        <f>(4030 * 3) + (3425 * 9) + (10215 * 12) + (4830 * 12) + 567 + (2309 * 9)</f>
-        <v>244803</v>
+        <f>SUM(I3:I4) * 12 + I5 * 7</f>
+        <v>174204</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4">
-        <f>B43-C43</f>
-        <v>5197</v>
+        <f t="shared" si="0"/>
+        <v>75796</v>
       </c>
       <c r="F43" s="4"/>
-      <c r="G43">
-        <f>G37*0.1/12</f>
-        <v>2375</v>
-      </c>
-      <c r="H43" s="20">
-        <v>9</v>
-      </c>
-      <c r="I43" s="20">
-        <f>G43*H43</f>
-        <v>21375</v>
-      </c>
-      <c r="J43" s="43">
-        <f>C43+I43</f>
-        <v>266178</v>
-      </c>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="40"/>
       <c r="K43" s="3"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
@@ -2335,26 +2327,16 @@
       <c r="U43" s="4"/>
     </row>
     <row r="44" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A44" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="4">
-        <v>250000</v>
-      </c>
-      <c r="C44" s="4">
-        <f>SUM(I3:I5) * 12 + I6 * 7</f>
-        <v>188712</v>
-      </c>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
       <c r="D44" s="4"/>
-      <c r="E44" s="4">
-        <f t="shared" si="0"/>
-        <v>61288</v>
-      </c>
+      <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="45"/>
+      <c r="J44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
@@ -2460,7 +2442,7 @@
       <c r="U48" s="4"/>
     </row>
     <row r="49" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A49" s="4"/>
+      <c r="A49" s="38"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
@@ -2483,7 +2465,7 @@
       <c r="U49" s="4"/>
     </row>
     <row r="50" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A50" s="43"/>
+      <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -3816,29 +3798,6 @@
       <c r="T107" s="4"/>
       <c r="U107" s="4"/>
     </row>
-    <row r="108" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A108" s="4"/>
-      <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="4"/>
-      <c r="G108" s="4"/>
-      <c r="H108" s="4"/>
-      <c r="I108" s="4"/>
-      <c r="J108" s="3"/>
-      <c r="K108" s="3"/>
-      <c r="L108" s="4"/>
-      <c r="M108" s="4"/>
-      <c r="N108" s="4"/>
-      <c r="O108" s="4"/>
-      <c r="P108" s="4"/>
-      <c r="Q108" s="4"/>
-      <c r="R108" s="4"/>
-      <c r="S108" s="4"/>
-      <c r="T108" s="4"/>
-      <c r="U108" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>